<commit_message>
fixed TIME_INTERVAL value in server.js
</commit_message>
<xml_diff>
--- a/back_end/tmp_data/2018_2019_FoI Class Feedback Form (Responses).xlsx
+++ b/back_end/tmp_data/2018_2019_FoI Class Feedback Form (Responses).xlsx
@@ -8776,8 +8776,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="3" width="21.57"/>
-    <col customWidth="1" min="4" max="4" width="40.71"/>
-    <col customWidth="1" min="5" max="12" width="21.57"/>
+    <col customWidth="1" min="4" max="4" width="58.86"/>
+    <col customWidth="1" min="5" max="5" width="49.43"/>
+    <col customWidth="1" min="6" max="12" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>